<commit_message>
10/17/19 New work files, ToDo for JM, PowerShell Script for installed Win Apps
</commit_message>
<xml_diff>
--- a/CurrentWork_Delta/PAD_hCentive/DDCA QA State Sales Platform hCentive PAD - Current State.xlsx
+++ b/CurrentWork_Delta/PAD_hCentive/DDCA QA State Sales Platform hCentive PAD - Current State.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BAEC87-9E8E-44DA-9BD5-C53870E86F64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5CA23A-2BB6-4EA0-B35C-BE7BDE036A06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30885" yWindow="1980" windowWidth="21600" windowHeight="13350" tabRatio="513" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2715" yWindow="960" windowWidth="27240" windowHeight="13170" tabRatio="513" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="3" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'QE PreState'!$A$3:$O$3</definedName>
-    <definedName name="_xlcn.WorksheetConnection_WorksheetA3I831" hidden="1">[1]Worksheet!$A$3:$I$84</definedName>
-    <definedName name="_xlcn.WorksheetConnection_WorksheetA5I831" hidden="1">[1]Worksheet!$A$5:$I$84</definedName>
+    <definedName name="_xlcn.WorksheetConnection_WorksheetA3I83" hidden="1">[1]Worksheet!$A$3:$I$84</definedName>
+    <definedName name="_xlcn.WorksheetConnection_WorksheetA5I83" hidden="1">[1]Worksheet!$A$5:$I$84</definedName>
     <definedName name="LEVELS">Lookup!$A$1:$C$5</definedName>
     <definedName name="SCORE">Lookup!$B$1:$C$5</definedName>
   </definedNames>
@@ -63,7 +63,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_WorksheetA3I831"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_WorksheetA3I83"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -72,7 +72,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range 1" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_WorksheetA5I831"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_WorksheetA5I83"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -2446,48 +2446,6 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
@@ -2495,6 +2453,48 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4632,24 +4632,22 @@
   <dimension ref="A1:O114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
+      <pane ySplit="3" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="21" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="21" customWidth="1"/>
+    <col min="5" max="6" width="14.85546875" style="31" customWidth="1"/>
+    <col min="7" max="8" width="24.7109375" style="31" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" style="21" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" style="21" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" style="39" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="39" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" style="21" customWidth="1"/>
     <col min="13" max="13" width="95.5703125" style="21" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" style="21" bestFit="1"/>
     <col min="15" max="15" width="12" style="21" bestFit="1" customWidth="1"/>
@@ -4739,8 +4737,8 @@
       <c r="M4" s="86"/>
     </row>
     <row r="5" spans="1:15" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
-      <c r="B5" s="100" t="s">
+      <c r="A5" s="102"/>
+      <c r="B5" s="103" t="s">
         <v>120</v>
       </c>
       <c r="C5" s="55" t="s">
@@ -4778,8 +4776,8 @@
       <c r="O5" s="19"/>
     </row>
     <row r="6" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
-      <c r="B6" s="101"/>
+      <c r="A6" s="102"/>
+      <c r="B6" s="104"/>
       <c r="C6" s="34" t="s">
         <v>411</v>
       </c>
@@ -4812,8 +4810,8 @@
       <c r="O6" s="19"/>
     </row>
     <row r="7" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="99"/>
-      <c r="B7" s="101"/>
+      <c r="A7" s="102"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="34" t="s">
         <v>85</v>
       </c>
@@ -4845,8 +4843,8 @@
       <c r="N7" s="41"/>
     </row>
     <row r="8" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="99"/>
-      <c r="B8" s="101"/>
+      <c r="A8" s="102"/>
+      <c r="B8" s="104"/>
       <c r="C8" s="17" t="s">
         <v>319</v>
       </c>
@@ -4878,8 +4876,8 @@
       <c r="N8" s="41"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
-      <c r="B9" s="101"/>
+      <c r="A9" s="102"/>
+      <c r="B9" s="104"/>
       <c r="C9" s="17" t="s">
         <v>70</v>
       </c>
@@ -4912,8 +4910,8 @@
       <c r="O9" s="19"/>
     </row>
     <row r="10" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="99"/>
-      <c r="B10" s="101"/>
+      <c r="A10" s="102"/>
+      <c r="B10" s="104"/>
       <c r="C10" s="17" t="s">
         <v>329</v>
       </c>
@@ -4945,8 +4943,8 @@
       <c r="N10" s="41"/>
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="99"/>
-      <c r="B11" s="101"/>
+      <c r="A11" s="102"/>
+      <c r="B11" s="104"/>
       <c r="C11" s="17" t="s">
         <v>328</v>
       </c>
@@ -4979,8 +4977,8 @@
       <c r="N11" s="41"/>
     </row>
     <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="99"/>
-      <c r="B12" s="101"/>
+      <c r="A12" s="102"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="17" t="s">
         <v>397</v>
       </c>
@@ -5013,8 +5011,8 @@
       <c r="N12" s="41"/>
     </row>
     <row r="13" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="99"/>
-      <c r="B13" s="101"/>
+      <c r="A13" s="102"/>
+      <c r="B13" s="104"/>
       <c r="C13" s="34" t="s">
         <v>428</v>
       </c>
@@ -5048,8 +5046,8 @@
       <c r="N13" s="41"/>
     </row>
     <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="99"/>
-      <c r="B14" s="101"/>
+      <c r="A14" s="102"/>
+      <c r="B14" s="104"/>
       <c r="C14" s="17" t="s">
         <v>324</v>
       </c>
@@ -5074,8 +5072,8 @@
       <c r="N14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="99"/>
-      <c r="B15" s="101"/>
+      <c r="A15" s="102"/>
+      <c r="B15" s="104"/>
       <c r="C15" s="34" t="s">
         <v>330</v>
       </c>
@@ -5108,9 +5106,9 @@
       </c>
       <c r="N15" s="41"/>
     </row>
-    <row r="16" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="99"/>
-      <c r="B16" s="101"/>
+    <row r="16" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="102"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="34" t="s">
         <v>422</v>
       </c>
@@ -5143,9 +5141,9 @@
       </c>
       <c r="N16" s="41"/>
     </row>
-    <row r="17" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="99"/>
-      <c r="B17" s="101"/>
+    <row r="17" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="102"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="34" t="s">
         <v>331</v>
       </c>
@@ -5179,8 +5177,8 @@
       <c r="N17" s="41"/>
     </row>
     <row r="18" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="99"/>
-      <c r="B18" s="102"/>
+      <c r="A18" s="102"/>
+      <c r="B18" s="105"/>
       <c r="C18" s="60" t="s">
         <v>129</v>
       </c>
@@ -5214,8 +5212,8 @@
       <c r="N18" s="41"/>
     </row>
     <row r="19" spans="1:15" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="99"/>
-      <c r="B19" s="100" t="s">
+      <c r="A19" s="102"/>
+      <c r="B19" s="103" t="s">
         <v>392</v>
       </c>
       <c r="C19" s="55" t="s">
@@ -5254,8 +5252,8 @@
       <c r="O19" s="19"/>
     </row>
     <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="99"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="102"/>
+      <c r="B20" s="104"/>
       <c r="C20" s="24" t="s">
         <v>335</v>
       </c>
@@ -5289,8 +5287,8 @@
       <c r="N20" s="41"/>
     </row>
     <row r="21" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="99"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="102"/>
+      <c r="B21" s="104"/>
       <c r="C21" s="17" t="s">
         <v>157</v>
       </c>
@@ -5322,8 +5320,8 @@
       <c r="N21" s="41"/>
     </row>
     <row r="22" spans="1:15" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="99"/>
-      <c r="B22" s="102"/>
+      <c r="A22" s="102"/>
+      <c r="B22" s="105"/>
       <c r="C22" s="89" t="s">
         <v>162</v>
       </c>
@@ -5354,8 +5352,8 @@
       <c r="N22" s="41"/>
     </row>
     <row r="23" spans="1:15" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="99"/>
-      <c r="B23" s="100" t="s">
+      <c r="A23" s="102"/>
+      <c r="B23" s="103" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="55" t="s">
@@ -5398,8 +5396,8 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="99"/>
-      <c r="B24" s="101"/>
+      <c r="A24" s="102"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="17" t="s">
         <v>86</v>
       </c>
@@ -5432,8 +5430,8 @@
       <c r="O24" s="19"/>
     </row>
     <row r="25" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="99"/>
-      <c r="B25" s="102"/>
+      <c r="A25" s="102"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="60" t="s">
         <v>87</v>
       </c>
@@ -5468,8 +5466,8 @@
       <c r="O25" s="19"/>
     </row>
     <row r="26" spans="1:15" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="99"/>
-      <c r="B26" s="100" t="s">
+      <c r="A26" s="102"/>
+      <c r="B26" s="103" t="s">
         <v>101</v>
       </c>
       <c r="C26" s="65" t="s">
@@ -5509,8 +5507,8 @@
       <c r="O26" s="19"/>
     </row>
     <row r="27" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="99"/>
-      <c r="B27" s="101"/>
+      <c r="A27" s="102"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="17" t="s">
         <v>362</v>
       </c>
@@ -5544,8 +5542,8 @@
       <c r="N27" s="41"/>
     </row>
     <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="99"/>
-      <c r="B28" s="101"/>
+      <c r="A28" s="102"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="17" t="s">
         <v>123</v>
       </c>
@@ -5577,8 +5575,8 @@
       <c r="N28" s="41"/>
     </row>
     <row r="29" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="99"/>
-      <c r="B29" s="101"/>
+      <c r="A29" s="102"/>
+      <c r="B29" s="104"/>
       <c r="C29" s="17" t="s">
         <v>146</v>
       </c>
@@ -5610,8 +5608,8 @@
       <c r="N29" s="41"/>
     </row>
     <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="99"/>
-      <c r="B30" s="101"/>
+      <c r="A30" s="102"/>
+      <c r="B30" s="104"/>
       <c r="C30" s="96" t="s">
         <v>242</v>
       </c>
@@ -5643,8 +5641,8 @@
       <c r="N30" s="41"/>
     </row>
     <row r="31" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="99"/>
-      <c r="B31" s="101"/>
+      <c r="A31" s="102"/>
+      <c r="B31" s="104"/>
       <c r="C31" s="34" t="s">
         <v>434</v>
       </c>
@@ -5678,8 +5676,8 @@
       <c r="N31" s="41"/>
     </row>
     <row r="32" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A32" s="99"/>
-      <c r="B32" s="101"/>
+      <c r="A32" s="102"/>
+      <c r="B32" s="104"/>
       <c r="C32" s="34" t="s">
         <v>404</v>
       </c>
@@ -5713,8 +5711,8 @@
       <c r="N32" s="41"/>
     </row>
     <row r="33" spans="1:15" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="99"/>
-      <c r="B33" s="102"/>
+      <c r="A33" s="102"/>
+      <c r="B33" s="105"/>
       <c r="C33" s="35" t="s">
         <v>493</v>
       </c>
@@ -5748,8 +5746,8 @@
       <c r="N33" s="41"/>
     </row>
     <row r="34" spans="1:15" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="99"/>
-      <c r="B34" s="100" t="s">
+      <c r="A34" s="102"/>
+      <c r="B34" s="103" t="s">
         <v>147</v>
       </c>
       <c r="C34" s="55" t="s">
@@ -5786,8 +5784,8 @@
       <c r="N34" s="41"/>
     </row>
     <row r="35" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="99"/>
-      <c r="B35" s="101"/>
+      <c r="A35" s="102"/>
+      <c r="B35" s="104"/>
       <c r="C35" s="17" t="s">
         <v>281</v>
       </c>
@@ -5819,8 +5817,8 @@
       <c r="N35" s="41"/>
     </row>
     <row r="36" spans="1:15" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="99"/>
-      <c r="B36" s="102"/>
+      <c r="A36" s="102"/>
+      <c r="B36" s="105"/>
       <c r="C36" s="77" t="s">
         <v>255</v>
       </c>
@@ -5852,8 +5850,8 @@
       <c r="N36" s="41"/>
     </row>
     <row r="37" spans="1:15" ht="111.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="99"/>
-      <c r="B37" s="100" t="s">
+      <c r="A37" s="102"/>
+      <c r="B37" s="103" t="s">
         <v>148</v>
       </c>
       <c r="C37" s="34" t="s">
@@ -5874,7 +5872,7 @@
       <c r="H37" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="I37" s="113" t="s">
+      <c r="I37" s="99" t="s">
         <v>6</v>
       </c>
       <c r="J37" s="56">
@@ -5892,8 +5890,8 @@
       <c r="N37" s="41"/>
     </row>
     <row r="38" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="99"/>
-      <c r="B38" s="101"/>
+      <c r="A38" s="102"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="34" t="s">
         <v>266</v>
       </c>
@@ -5925,8 +5923,8 @@
       <c r="N38" s="41"/>
     </row>
     <row r="39" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="99"/>
-      <c r="B39" s="102"/>
+      <c r="A39" s="102"/>
+      <c r="B39" s="105"/>
       <c r="C39" s="60" t="s">
         <v>186</v>
       </c>
@@ -5958,8 +5956,8 @@
       <c r="N39" s="41"/>
     </row>
     <row r="40" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="99"/>
-      <c r="B40" s="104" t="s">
+      <c r="A40" s="102"/>
+      <c r="B40" s="106" t="s">
         <v>10</v>
       </c>
       <c r="C40" s="55" t="s">
@@ -6000,8 +5998,8 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="99"/>
-      <c r="B41" s="104"/>
+      <c r="A41" s="102"/>
+      <c r="B41" s="106"/>
       <c r="C41" s="17" t="s">
         <v>17</v>
       </c>
@@ -6035,8 +6033,8 @@
       <c r="N41" s="41"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="99"/>
-      <c r="B42" s="104"/>
+      <c r="A42" s="102"/>
+      <c r="B42" s="106"/>
       <c r="C42" s="17" t="s">
         <v>22</v>
       </c>
@@ -6068,8 +6066,8 @@
       <c r="N42" s="41"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="99"/>
-      <c r="B43" s="104"/>
+      <c r="A43" s="102"/>
+      <c r="B43" s="106"/>
       <c r="C43" s="17" t="s">
         <v>27</v>
       </c>
@@ -6103,8 +6101,8 @@
       <c r="N43" s="41"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="99"/>
-      <c r="B44" s="104"/>
+      <c r="A44" s="102"/>
+      <c r="B44" s="106"/>
       <c r="C44" s="17" t="s">
         <v>32</v>
       </c>
@@ -6136,8 +6134,8 @@
       <c r="N44" s="41"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="99"/>
-      <c r="B45" s="104"/>
+      <c r="A45" s="102"/>
+      <c r="B45" s="106"/>
       <c r="C45" s="42" t="s">
         <v>37</v>
       </c>
@@ -6169,8 +6167,8 @@
       <c r="N45" s="41"/>
     </row>
     <row r="46" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="99"/>
-      <c r="B46" s="104" t="s">
+      <c r="A46" s="102"/>
+      <c r="B46" s="106" t="s">
         <v>81</v>
       </c>
       <c r="C46" s="34" t="s">
@@ -6210,8 +6208,8 @@
       <c r="O46" s="19"/>
     </row>
     <row r="47" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="99"/>
-      <c r="B47" s="104"/>
+      <c r="A47" s="102"/>
+      <c r="B47" s="106"/>
       <c r="C47" s="34" t="s">
         <v>400</v>
       </c>
@@ -6244,8 +6242,8 @@
       <c r="O47" s="19"/>
     </row>
     <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="99"/>
-      <c r="B48" s="104"/>
+      <c r="A48" s="102"/>
+      <c r="B48" s="106"/>
       <c r="C48" s="17" t="s">
         <v>300</v>
       </c>
@@ -6278,8 +6276,8 @@
       <c r="O48" s="19"/>
     </row>
     <row r="49" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="99"/>
-      <c r="B49" s="104"/>
+      <c r="A49" s="102"/>
+      <c r="B49" s="106"/>
       <c r="C49" s="17" t="s">
         <v>295</v>
       </c>
@@ -6312,8 +6310,8 @@
       <c r="O49" s="19"/>
     </row>
     <row r="50" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" s="99"/>
-      <c r="B50" s="104"/>
+      <c r="A50" s="102"/>
+      <c r="B50" s="106"/>
       <c r="C50" s="34" t="s">
         <v>393</v>
       </c>
@@ -6348,8 +6346,8 @@
       <c r="O50" s="19"/>
     </row>
     <row r="51" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="99"/>
-      <c r="B51" s="104"/>
+      <c r="A51" s="102"/>
+      <c r="B51" s="106"/>
       <c r="C51" s="34" t="s">
         <v>261</v>
       </c>
@@ -6384,8 +6382,8 @@
       <c r="O51" s="19"/>
     </row>
     <row r="52" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="99"/>
-      <c r="B52" s="104"/>
+      <c r="A52" s="102"/>
+      <c r="B52" s="106"/>
       <c r="C52" s="17" t="s">
         <v>46</v>
       </c>
@@ -6417,8 +6415,8 @@
       <c r="N52" s="41"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="99"/>
-      <c r="B53" s="104"/>
+      <c r="A53" s="102"/>
+      <c r="B53" s="106"/>
       <c r="C53" s="17" t="s">
         <v>437</v>
       </c>
@@ -6449,8 +6447,8 @@
       <c r="N53" s="41"/>
     </row>
     <row r="54" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="99"/>
-      <c r="B54" s="104"/>
+      <c r="A54" s="102"/>
+      <c r="B54" s="106"/>
       <c r="C54" s="17" t="s">
         <v>55</v>
       </c>
@@ -6482,8 +6480,8 @@
       <c r="N54" s="41"/>
     </row>
     <row r="55" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="99"/>
-      <c r="B55" s="104"/>
+      <c r="A55" s="102"/>
+      <c r="B55" s="106"/>
       <c r="C55" s="17" t="s">
         <v>60</v>
       </c>
@@ -6517,8 +6515,8 @@
       <c r="N55" s="41"/>
     </row>
     <row r="56" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="99"/>
-      <c r="B56" s="104"/>
+      <c r="A56" s="102"/>
+      <c r="B56" s="106"/>
       <c r="C56" s="34" t="s">
         <v>469</v>
       </c>
@@ -6552,8 +6550,8 @@
       <c r="N56" s="41"/>
     </row>
     <row r="57" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="99"/>
-      <c r="B57" s="104"/>
+      <c r="A57" s="102"/>
+      <c r="B57" s="106"/>
       <c r="C57" s="17" t="s">
         <v>471</v>
       </c>
@@ -6585,8 +6583,8 @@
       <c r="N57" s="41"/>
     </row>
     <row r="58" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="99"/>
-      <c r="B58" s="104"/>
+      <c r="A58" s="102"/>
+      <c r="B58" s="106"/>
       <c r="C58" s="17" t="s">
         <v>106</v>
       </c>
@@ -6618,8 +6616,8 @@
       <c r="N58" s="41"/>
     </row>
     <row r="59" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="99"/>
-      <c r="B59" s="104"/>
+      <c r="A59" s="102"/>
+      <c r="B59" s="106"/>
       <c r="C59" s="17" t="s">
         <v>111</v>
       </c>
@@ -6651,8 +6649,8 @@
       <c r="N59" s="41"/>
     </row>
     <row r="60" spans="1:15" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="99"/>
-      <c r="B60" s="105"/>
+      <c r="A60" s="102"/>
+      <c r="B60" s="107"/>
       <c r="C60" s="17" t="s">
         <v>80</v>
       </c>
@@ -6686,8 +6684,8 @@
       <c r="N60" s="41"/>
     </row>
     <row r="61" spans="1:15" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="99"/>
-      <c r="B61" s="106" t="s">
+      <c r="A61" s="102"/>
+      <c r="B61" s="108" t="s">
         <v>134</v>
       </c>
       <c r="C61" s="55" t="s">
@@ -6728,8 +6726,8 @@
       </c>
     </row>
     <row r="62" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="99"/>
-      <c r="B62" s="104"/>
+      <c r="A62" s="102"/>
+      <c r="B62" s="106"/>
       <c r="C62" s="17" t="s">
         <v>438</v>
       </c>
@@ -6762,8 +6760,8 @@
       <c r="O62" s="19"/>
     </row>
     <row r="63" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="99"/>
-      <c r="B63" s="104"/>
+      <c r="A63" s="102"/>
+      <c r="B63" s="106"/>
       <c r="C63" s="17" t="s">
         <v>444</v>
       </c>
@@ -6790,8 +6788,8 @@
       <c r="O63" s="19"/>
     </row>
     <row r="64" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="99"/>
-      <c r="B64" s="104"/>
+      <c r="A64" s="102"/>
+      <c r="B64" s="106"/>
       <c r="C64" s="17" t="s">
         <v>287</v>
       </c>
@@ -6818,8 +6816,8 @@
       <c r="O64" s="19"/>
     </row>
     <row r="65" spans="1:15" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="99"/>
-      <c r="B65" s="107"/>
+      <c r="A65" s="102"/>
+      <c r="B65" s="109"/>
       <c r="C65" s="89" t="s">
         <v>346</v>
       </c>
@@ -6852,8 +6850,8 @@
       <c r="O65" s="19"/>
     </row>
     <row r="66" spans="1:15" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="99"/>
-      <c r="B66" s="105"/>
+      <c r="A66" s="102"/>
+      <c r="B66" s="107"/>
       <c r="C66" s="89" t="s">
         <v>530</v>
       </c>
@@ -6887,8 +6885,8 @@
       <c r="N66" s="41"/>
     </row>
     <row r="67" spans="1:15" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="99"/>
-      <c r="B67" s="106" t="s">
+      <c r="A67" s="102"/>
+      <c r="B67" s="108" t="s">
         <v>207</v>
       </c>
       <c r="C67" s="55" t="s">
@@ -6929,8 +6927,8 @@
       </c>
     </row>
     <row r="68" spans="1:15" ht="150" x14ac:dyDescent="0.25">
-      <c r="A68" s="99"/>
-      <c r="B68" s="104"/>
+      <c r="A68" s="102"/>
+      <c r="B68" s="106"/>
       <c r="C68" s="17" t="s">
         <v>212</v>
       </c>
@@ -6962,8 +6960,8 @@
       <c r="N68" s="41"/>
     </row>
     <row r="69" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="99"/>
-      <c r="B69" s="104"/>
+      <c r="A69" s="102"/>
+      <c r="B69" s="106"/>
       <c r="C69" s="17" t="s">
         <v>214</v>
       </c>
@@ -6995,8 +6993,8 @@
       <c r="N69" s="41"/>
     </row>
     <row r="70" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="99"/>
-      <c r="B70" s="105"/>
+      <c r="A70" s="102"/>
+      <c r="B70" s="107"/>
       <c r="C70" s="60" t="s">
         <v>219</v>
       </c>
@@ -7015,7 +7013,7 @@
       <c r="H70" s="62" t="s">
         <v>228</v>
       </c>
-      <c r="I70" s="114" t="s">
+      <c r="I70" s="100" t="s">
         <v>5</v>
       </c>
       <c r="J70" s="61">
@@ -7030,7 +7028,7 @@
       <c r="N70" s="41"/>
     </row>
     <row r="71" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="99"/>
+      <c r="A71" s="102"/>
       <c r="B71" s="53"/>
       <c r="C71" s="48"/>
       <c r="D71" s="49"/>
@@ -7046,19 +7044,19 @@
       <c r="N71" s="41"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="99"/>
-      <c r="B72" s="103"/>
-      <c r="C72" s="103"/>
-      <c r="D72" s="103"/>
-      <c r="E72" s="103"/>
-      <c r="F72" s="103"/>
-      <c r="G72" s="103"/>
-      <c r="H72" s="103"/>
-      <c r="I72" s="103"/>
-      <c r="J72" s="103"/>
-      <c r="K72" s="103"/>
-      <c r="L72" s="103"/>
-      <c r="M72" s="103"/>
+      <c r="A72" s="102"/>
+      <c r="B72" s="101"/>
+      <c r="C72" s="101"/>
+      <c r="D72" s="101"/>
+      <c r="E72" s="101"/>
+      <c r="F72" s="101"/>
+      <c r="G72" s="101"/>
+      <c r="H72" s="101"/>
+      <c r="I72" s="101"/>
+      <c r="J72" s="101"/>
+      <c r="K72" s="101"/>
+      <c r="L72" s="101"/>
+      <c r="M72" s="101"/>
       <c r="N72" s="41"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
@@ -7231,6 +7229,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A5:A22"/>
+    <mergeCell ref="B5:B18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
     <mergeCell ref="B72:M72"/>
     <mergeCell ref="A26:A33"/>
     <mergeCell ref="B26:B33"/>
@@ -7242,11 +7245,6 @@
     <mergeCell ref="B46:B60"/>
     <mergeCell ref="B61:B66"/>
     <mergeCell ref="B67:B70"/>
-    <mergeCell ref="A5:A22"/>
-    <mergeCell ref="B5:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
   </mergeCells>
   <conditionalFormatting sqref="B23">
     <cfRule type="expression" dxfId="87" priority="45" stopIfTrue="1">
@@ -7755,8 +7753,8 @@
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="108"/>
-      <c r="B5" s="109" t="s">
+      <c r="A5" s="110"/>
+      <c r="B5" s="111" t="s">
         <v>120</v>
       </c>
       <c r="C5" s="23" t="s">
@@ -7791,8 +7789,8 @@
       <c r="O5" s="19"/>
     </row>
     <row r="6" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="108"/>
-      <c r="B6" s="109"/>
+      <c r="A6" s="110"/>
+      <c r="B6" s="111"/>
       <c r="C6" s="23" t="s">
         <v>85</v>
       </c>
@@ -7824,8 +7822,8 @@
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="108"/>
-      <c r="B7" s="109"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="111"/>
       <c r="C7" s="23" t="s">
         <v>319</v>
       </c>
@@ -7857,8 +7855,8 @@
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="108"/>
-      <c r="B8" s="109"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="111"/>
       <c r="C8" s="17" t="s">
         <v>70</v>
       </c>
@@ -7890,8 +7888,8 @@
       <c r="O8" s="19"/>
     </row>
     <row r="9" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="108"/>
-      <c r="B9" s="109"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="111"/>
       <c r="C9" s="17" t="s">
         <v>329</v>
       </c>
@@ -7925,8 +7923,8 @@
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="108"/>
-      <c r="B10" s="109"/>
+      <c r="A10" s="110"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="17" t="s">
         <v>328</v>
       </c>
@@ -7959,8 +7957,8 @@
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="108"/>
-      <c r="B11" s="109"/>
+      <c r="A11" s="110"/>
+      <c r="B11" s="111"/>
       <c r="C11" s="17" t="s">
         <v>355</v>
       </c>
@@ -7993,8 +7991,8 @@
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="108"/>
-      <c r="B12" s="109"/>
+      <c r="A12" s="110"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="17" t="s">
         <v>309</v>
       </c>
@@ -8028,8 +8026,8 @@
       <c r="N12" s="7"/>
     </row>
     <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="108"/>
-      <c r="B13" s="109"/>
+      <c r="A13" s="110"/>
+      <c r="B13" s="111"/>
       <c r="C13" s="23" t="s">
         <v>324</v>
       </c>
@@ -8054,8 +8052,8 @@
       <c r="N13" s="7"/>
     </row>
     <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="108"/>
-      <c r="B14" s="109"/>
+      <c r="A14" s="110"/>
+      <c r="B14" s="111"/>
       <c r="C14" s="17" t="s">
         <v>330</v>
       </c>
@@ -8086,8 +8084,8 @@
       <c r="N14" s="7"/>
     </row>
     <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="108"/>
-      <c r="B15" s="109"/>
+      <c r="A15" s="110"/>
+      <c r="B15" s="111"/>
       <c r="C15" s="17" t="s">
         <v>331</v>
       </c>
@@ -8121,8 +8119,8 @@
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="108"/>
-      <c r="B16" s="109"/>
+      <c r="A16" s="110"/>
+      <c r="B16" s="111"/>
       <c r="C16" s="17" t="s">
         <v>129</v>
       </c>
@@ -8156,8 +8154,8 @@
       <c r="N16" s="7"/>
     </row>
     <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="108"/>
-      <c r="B17" s="109" t="s">
+      <c r="A17" s="110"/>
+      <c r="B17" s="111" t="s">
         <v>100</v>
       </c>
       <c r="C17" s="17" t="s">
@@ -8194,8 +8192,8 @@
       <c r="O17" s="19"/>
     </row>
     <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="108"/>
-      <c r="B18" s="109"/>
+      <c r="A18" s="110"/>
+      <c r="B18" s="111"/>
       <c r="C18" s="17" t="s">
         <v>117</v>
       </c>
@@ -8226,8 +8224,8 @@
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="108"/>
-      <c r="B19" s="109"/>
+      <c r="A19" s="110"/>
+      <c r="B19" s="111"/>
       <c r="C19" s="17" t="s">
         <v>149</v>
       </c>
@@ -8258,8 +8256,8 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="108"/>
-      <c r="B20" s="109" t="s">
+      <c r="A20" s="110"/>
+      <c r="B20" s="111" t="s">
         <v>102</v>
       </c>
       <c r="C20" s="17" t="s">
@@ -8299,8 +8297,8 @@
       <c r="O20" s="19"/>
     </row>
     <row r="21" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="108"/>
-      <c r="B21" s="109"/>
+      <c r="A21" s="110"/>
+      <c r="B21" s="111"/>
       <c r="C21" s="24" t="s">
         <v>335</v>
       </c>
@@ -8331,8 +8329,8 @@
       <c r="N21" s="7"/>
     </row>
     <row r="22" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="108"/>
-      <c r="B22" s="109"/>
+      <c r="A22" s="110"/>
+      <c r="B22" s="111"/>
       <c r="C22" s="17" t="s">
         <v>157</v>
       </c>
@@ -8366,8 +8364,8 @@
       <c r="N22" s="7"/>
     </row>
     <row r="23" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="108"/>
-      <c r="B23" s="109"/>
+      <c r="A23" s="110"/>
+      <c r="B23" s="111"/>
       <c r="C23" s="17" t="s">
         <v>162</v>
       </c>
@@ -8401,8 +8399,8 @@
       <c r="N23" s="7"/>
     </row>
     <row r="24" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="108"/>
-      <c r="B24" s="109" t="s">
+      <c r="A24" s="110"/>
+      <c r="B24" s="111" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="25" t="s">
@@ -8444,8 +8442,8 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="108"/>
-      <c r="B25" s="109"/>
+      <c r="A25" s="110"/>
+      <c r="B25" s="111"/>
       <c r="C25" s="25" t="s">
         <v>86</v>
       </c>
@@ -8476,8 +8474,8 @@
       <c r="O25" s="19"/>
     </row>
     <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="108"/>
-      <c r="B26" s="109"/>
+      <c r="A26" s="110"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="25" t="s">
         <v>104</v>
       </c>
@@ -8511,8 +8509,8 @@
       <c r="O26" s="19"/>
     </row>
     <row r="27" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="108"/>
-      <c r="B27" s="109"/>
+      <c r="A27" s="110"/>
+      <c r="B27" s="111"/>
       <c r="C27" s="25" t="s">
         <v>87</v>
       </c>
@@ -8546,8 +8544,8 @@
       <c r="O27" s="19"/>
     </row>
     <row r="28" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="108"/>
-      <c r="B28" s="109" t="s">
+      <c r="A28" s="110"/>
+      <c r="B28" s="111" t="s">
         <v>101</v>
       </c>
       <c r="C28" s="17" t="s">
@@ -8584,8 +8582,8 @@
       <c r="O28" s="19"/>
     </row>
     <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="108"/>
-      <c r="B29" s="109"/>
+      <c r="A29" s="110"/>
+      <c r="B29" s="111"/>
       <c r="C29" s="17" t="s">
         <v>362</v>
       </c>
@@ -8619,8 +8617,8 @@
       <c r="N29" s="7"/>
     </row>
     <row r="30" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="108"/>
-      <c r="B30" s="109"/>
+      <c r="A30" s="110"/>
+      <c r="B30" s="111"/>
       <c r="C30" s="17" t="s">
         <v>123</v>
       </c>
@@ -8651,8 +8649,8 @@
       <c r="N30" s="7"/>
     </row>
     <row r="31" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="108"/>
-      <c r="B31" s="109"/>
+      <c r="A31" s="110"/>
+      <c r="B31" s="111"/>
       <c r="C31" s="17" t="s">
         <v>146</v>
       </c>
@@ -8683,8 +8681,8 @@
       <c r="N31" s="7"/>
     </row>
     <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="108"/>
-      <c r="B32" s="109"/>
+      <c r="A32" s="110"/>
+      <c r="B32" s="111"/>
       <c r="C32" s="17" t="s">
         <v>242</v>
       </c>
@@ -8715,8 +8713,8 @@
       <c r="N32" s="7"/>
     </row>
     <row r="33" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="108"/>
-      <c r="B33" s="109"/>
+      <c r="A33" s="110"/>
+      <c r="B33" s="111"/>
       <c r="C33" s="17" t="s">
         <v>249</v>
       </c>
@@ -8750,8 +8748,8 @@
       <c r="N33" s="7"/>
     </row>
     <row r="34" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="108"/>
-      <c r="B34" s="109"/>
+      <c r="A34" s="110"/>
+      <c r="B34" s="111"/>
       <c r="C34" s="17" t="s">
         <v>239</v>
       </c>
@@ -8782,8 +8780,8 @@
       <c r="N34" s="7"/>
     </row>
     <row r="35" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="108"/>
-      <c r="B35" s="109" t="s">
+      <c r="A35" s="110"/>
+      <c r="B35" s="111" t="s">
         <v>147</v>
       </c>
       <c r="C35" s="17" t="s">
@@ -8816,8 +8814,8 @@
       <c r="N35" s="7"/>
     </row>
     <row r="36" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="108"/>
-      <c r="B36" s="109"/>
+      <c r="A36" s="110"/>
+      <c r="B36" s="111"/>
       <c r="C36" s="17" t="s">
         <v>281</v>
       </c>
@@ -8851,8 +8849,8 @@
       <c r="N36" s="7"/>
     </row>
     <row r="37" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="108"/>
-      <c r="B37" s="109"/>
+      <c r="A37" s="110"/>
+      <c r="B37" s="111"/>
       <c r="C37" s="17" t="s">
         <v>344</v>
       </c>
@@ -8886,8 +8884,8 @@
       <c r="N37" s="7"/>
     </row>
     <row r="38" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="108"/>
-      <c r="B38" s="109"/>
+      <c r="A38" s="110"/>
+      <c r="B38" s="111"/>
       <c r="C38" s="17" t="s">
         <v>255</v>
       </c>
@@ -8921,8 +8919,8 @@
       <c r="N38" s="7"/>
     </row>
     <row r="39" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="108"/>
-      <c r="B39" s="109" t="s">
+      <c r="A39" s="110"/>
+      <c r="B39" s="111" t="s">
         <v>148</v>
       </c>
       <c r="C39" s="17" t="s">
@@ -8958,8 +8956,8 @@
       <c r="N39" s="7"/>
     </row>
     <row r="40" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A40" s="108"/>
-      <c r="B40" s="109"/>
+      <c r="A40" s="110"/>
+      <c r="B40" s="111"/>
       <c r="C40" s="17" t="s">
         <v>266</v>
       </c>
@@ -8993,8 +8991,8 @@
       <c r="N40" s="7"/>
     </row>
     <row r="41" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="108"/>
-      <c r="B41" s="109"/>
+      <c r="A41" s="110"/>
+      <c r="B41" s="111"/>
       <c r="C41" s="17" t="s">
         <v>186</v>
       </c>
@@ -9025,8 +9023,8 @@
       <c r="N41" s="7"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="108"/>
-      <c r="B42" s="110" t="s">
+      <c r="A42" s="110"/>
+      <c r="B42" s="112" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="25" t="s">
@@ -9066,8 +9064,8 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="108"/>
-      <c r="B43" s="110"/>
+      <c r="A43" s="110"/>
+      <c r="B43" s="112"/>
       <c r="C43" s="25" t="s">
         <v>17</v>
       </c>
@@ -9098,8 +9096,8 @@
       <c r="M43" s="10"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="108"/>
-      <c r="B44" s="110"/>
+      <c r="A44" s="110"/>
+      <c r="B44" s="112"/>
       <c r="C44" s="25" t="s">
         <v>22</v>
       </c>
@@ -9130,8 +9128,8 @@
       <c r="M44" s="10"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="108"/>
-      <c r="B45" s="110"/>
+      <c r="A45" s="110"/>
+      <c r="B45" s="112"/>
       <c r="C45" s="25" t="s">
         <v>27</v>
       </c>
@@ -9162,8 +9160,8 @@
       <c r="M45" s="10"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="108"/>
-      <c r="B46" s="110"/>
+      <c r="A46" s="110"/>
+      <c r="B46" s="112"/>
       <c r="C46" s="25" t="s">
         <v>32</v>
       </c>
@@ -9194,8 +9192,8 @@
       <c r="M46" s="10"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="108"/>
-      <c r="B47" s="110"/>
+      <c r="A47" s="110"/>
+      <c r="B47" s="112"/>
       <c r="C47" s="25" t="s">
         <v>37</v>
       </c>
@@ -9226,8 +9224,8 @@
       <c r="M47" s="10"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="108"/>
-      <c r="B48" s="111" t="s">
+      <c r="A48" s="110"/>
+      <c r="B48" s="113" t="s">
         <v>81</v>
       </c>
       <c r="C48" s="17" t="s">
@@ -9264,8 +9262,8 @@
       <c r="O48" s="19"/>
     </row>
     <row r="49" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="108"/>
-      <c r="B49" s="111"/>
+      <c r="A49" s="110"/>
+      <c r="B49" s="113"/>
       <c r="C49" s="17" t="s">
         <v>300</v>
       </c>
@@ -9300,8 +9298,8 @@
       <c r="O49" s="19"/>
     </row>
     <row r="50" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="108"/>
-      <c r="B50" s="111"/>
+      <c r="A50" s="110"/>
+      <c r="B50" s="113"/>
       <c r="C50" s="17" t="s">
         <v>295</v>
       </c>
@@ -9336,8 +9334,8 @@
       <c r="O50" s="19"/>
     </row>
     <row r="51" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="108"/>
-      <c r="B51" s="111"/>
+      <c r="A51" s="110"/>
+      <c r="B51" s="113"/>
       <c r="C51" s="17" t="s">
         <v>261</v>
       </c>
@@ -9372,8 +9370,8 @@
       <c r="O51" s="19"/>
     </row>
     <row r="52" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="108"/>
-      <c r="B52" s="111"/>
+      <c r="A52" s="110"/>
+      <c r="B52" s="113"/>
       <c r="C52" s="17" t="s">
         <v>46</v>
       </c>
@@ -9404,8 +9402,8 @@
       <c r="N52" s="7"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="108"/>
-      <c r="B53" s="111"/>
+      <c r="A53" s="110"/>
+      <c r="B53" s="113"/>
       <c r="C53" s="17" t="s">
         <v>343</v>
       </c>
@@ -9435,8 +9433,8 @@
       <c r="N53" s="7"/>
     </row>
     <row r="54" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="108"/>
-      <c r="B54" s="111"/>
+      <c r="A54" s="110"/>
+      <c r="B54" s="113"/>
       <c r="C54" s="17" t="s">
         <v>55</v>
       </c>
@@ -9470,8 +9468,8 @@
       <c r="N54" s="7"/>
     </row>
     <row r="55" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="108"/>
-      <c r="B55" s="111"/>
+      <c r="A55" s="110"/>
+      <c r="B55" s="113"/>
       <c r="C55" s="17" t="s">
         <v>60</v>
       </c>
@@ -9505,8 +9503,8 @@
       <c r="N55" s="7"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="108"/>
-      <c r="B56" s="111"/>
+      <c r="A56" s="110"/>
+      <c r="B56" s="113"/>
       <c r="C56" s="17" t="s">
         <v>65</v>
       </c>
@@ -9540,8 +9538,8 @@
       <c r="N56" s="7"/>
     </row>
     <row r="57" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="108"/>
-      <c r="B57" s="111"/>
+      <c r="A57" s="110"/>
+      <c r="B57" s="113"/>
       <c r="C57" s="17" t="s">
         <v>106</v>
       </c>
@@ -9572,8 +9570,8 @@
       <c r="N57" s="7"/>
     </row>
     <row r="58" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="108"/>
-      <c r="B58" s="111"/>
+      <c r="A58" s="110"/>
+      <c r="B58" s="113"/>
       <c r="C58" s="17" t="s">
         <v>111</v>
       </c>
@@ -9607,8 +9605,8 @@
       <c r="N58" s="7"/>
     </row>
     <row r="59" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="108"/>
-      <c r="B59" s="111"/>
+      <c r="A59" s="110"/>
+      <c r="B59" s="113"/>
       <c r="C59" s="17" t="s">
         <v>80</v>
       </c>
@@ -9642,8 +9640,8 @@
       <c r="N59" s="7"/>
     </row>
     <row r="60" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="108"/>
-      <c r="B60" s="111" t="s">
+      <c r="A60" s="110"/>
+      <c r="B60" s="113" t="s">
         <v>134</v>
       </c>
       <c r="C60" s="25" t="s">
@@ -9685,8 +9683,8 @@
       </c>
     </row>
     <row r="61" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A61" s="108"/>
-      <c r="B61" s="111"/>
+      <c r="A61" s="110"/>
+      <c r="B61" s="113"/>
       <c r="C61" s="25" t="s">
         <v>290</v>
       </c>
@@ -9718,8 +9716,8 @@
       <c r="O61" s="19"/>
     </row>
     <row r="62" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="108"/>
-      <c r="B62" s="111"/>
+      <c r="A62" s="110"/>
+      <c r="B62" s="113"/>
       <c r="C62" s="25" t="s">
         <v>287</v>
       </c>
@@ -9749,8 +9747,8 @@
       <c r="O62" s="19"/>
     </row>
     <row r="63" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="108"/>
-      <c r="B63" s="111"/>
+      <c r="A63" s="110"/>
+      <c r="B63" s="113"/>
       <c r="C63" s="25" t="s">
         <v>346</v>
       </c>
@@ -9783,8 +9781,8 @@
       </c>
     </row>
     <row r="64" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A64" s="108"/>
-      <c r="B64" s="109" t="s">
+      <c r="A64" s="110"/>
+      <c r="B64" s="111" t="s">
         <v>207</v>
       </c>
       <c r="C64" s="25" t="s">
@@ -9824,8 +9822,8 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A65" s="108"/>
-      <c r="B65" s="111"/>
+      <c r="A65" s="110"/>
+      <c r="B65" s="113"/>
       <c r="C65" s="25" t="s">
         <v>212</v>
       </c>
@@ -9854,8 +9852,8 @@
       <c r="M65" s="10"/>
     </row>
     <row r="66" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="108"/>
-      <c r="B66" s="111"/>
+      <c r="A66" s="110"/>
+      <c r="B66" s="113"/>
       <c r="C66" s="25" t="s">
         <v>214</v>
       </c>
@@ -9886,8 +9884,8 @@
       <c r="M66" s="10"/>
     </row>
     <row r="67" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="108"/>
-      <c r="B67" s="111"/>
+      <c r="A67" s="110"/>
+      <c r="B67" s="113"/>
       <c r="C67" s="25" t="s">
         <v>219</v>
       </c>
@@ -9918,7 +9916,7 @@
       <c r="M67" s="10"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="108"/>
+      <c r="A68" s="110"/>
       <c r="B68" s="22"/>
       <c r="C68" s="25"/>
       <c r="D68" s="11"/>
@@ -9932,30 +9930,22 @@
       <c r="M68" s="10"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="108"/>
-      <c r="B69" s="112"/>
-      <c r="C69" s="112"/>
-      <c r="D69" s="112"/>
-      <c r="E69" s="112"/>
-      <c r="F69" s="112"/>
-      <c r="G69" s="112"/>
-      <c r="H69" s="112"/>
-      <c r="I69" s="112"/>
-      <c r="J69" s="112"/>
-      <c r="K69" s="112"/>
-      <c r="L69" s="112"/>
-      <c r="M69" s="112"/>
+      <c r="A69" s="110"/>
+      <c r="B69" s="114"/>
+      <c r="C69" s="114"/>
+      <c r="D69" s="114"/>
+      <c r="E69" s="114"/>
+      <c r="F69" s="114"/>
+      <c r="G69" s="114"/>
+      <c r="H69" s="114"/>
+      <c r="I69" s="114"/>
+      <c r="J69" s="114"/>
+      <c r="K69" s="114"/>
+      <c r="L69" s="114"/>
+      <c r="M69" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="A5:A23"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
     <mergeCell ref="A35:A41"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="A42:A69"/>
@@ -9965,6 +9955,14 @@
     <mergeCell ref="B64:B67"/>
     <mergeCell ref="B69:M69"/>
     <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="A5:A23"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
   </mergeCells>
   <conditionalFormatting sqref="B42">
     <cfRule type="expression" dxfId="43" priority="65" stopIfTrue="1">
@@ -10142,9 +10140,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10326,26 +10327,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B5D6DA9-DA9C-40FD-864E-7002926A1C0C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC436DC-1043-44B4-B2B1-062ADA839305}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1a832241-987a-4d79-9fcd-efb8bfe6011c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10369,9 +10359,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC436DC-1043-44B4-B2B1-062ADA839305}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B5D6DA9-DA9C-40FD-864E-7002926A1C0C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1a832241-987a-4d79-9fcd-efb8bfe6011c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>